<commit_message>
Change update scores logic to prevent displaying zeroes
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="F16" sqref="F16:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +706,78 @@
         <v>column44.setText(String.valueOf(board[3][3]));</v>
       </c>
     </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f>"if(board["&amp;LEFT(A1,1)-1&amp;"]["&amp;RIGHT(A1,1)-1&amp;"]!=0) "&amp;F11</f>
+        <v>if(board[0][0]!=0) column11.setText(String.valueOf(board[0][0]));</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ref="G16:I16" si="14">"if(board["&amp;LEFT(B1,1)-1&amp;"]["&amp;RIGHT(B1,1)-1&amp;"]!=0) "&amp;G11</f>
+        <v>if(board[0][1]!=0) column12.setText(String.valueOf(board[0][1]));</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="14"/>
+        <v>if(board[0][2]!=0) column13.setText(String.valueOf(board[0][2]));</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="14"/>
+        <v>if(board[0][3]!=0) column14.setText(String.valueOf(board[0][3]));</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" ref="F17:F19" si="15">"if(board["&amp;LEFT(A2,1)-1&amp;"]["&amp;RIGHT(A2,1)-1&amp;"]!=0) "&amp;F12</f>
+        <v>if(board[1][0]!=0) column21.setText(String.valueOf(board[1][0]));</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" ref="G17:G19" si="16">"if(board["&amp;LEFT(B2,1)-1&amp;"]["&amp;RIGHT(B2,1)-1&amp;"]!=0) "&amp;G12</f>
+        <v>if(board[1][1]!=0) column22.setText(String.valueOf(board[1][1]));</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" ref="H17:H19" si="17">"if(board["&amp;LEFT(C2,1)-1&amp;"]["&amp;RIGHT(C2,1)-1&amp;"]!=0) "&amp;H12</f>
+        <v>if(board[1][2]!=0) column23.setText(String.valueOf(board[1][2]));</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ref="I17:I19" si="18">"if(board["&amp;LEFT(D2,1)-1&amp;"]["&amp;RIGHT(D2,1)-1&amp;"]!=0) "&amp;I12</f>
+        <v>if(board[1][3]!=0) column24.setText(String.valueOf(board[1][3]));</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f t="shared" si="15"/>
+        <v>if(board[2][0]!=0) column31.setText(String.valueOf(board[2][0]));</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="16"/>
+        <v>if(board[2][1]!=0) column32.setText(String.valueOf(board[2][1]));</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="17"/>
+        <v>if(board[2][2]!=0) column33.setText(String.valueOf(board[2][2]));</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="18"/>
+        <v>if(board[2][3]!=0) column34.setText(String.valueOf(board[2][3]));</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="15"/>
+        <v>if(board[3][0]!=0) column41.setText(String.valueOf(board[3][0]));</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="16"/>
+        <v>if(board[3][1]!=0) column42.setText(String.valueOf(board[3][1]));</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="17"/>
+        <v>if(board[3][2]!=0) column43.setText(String.valueOf(board[3][2]));</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="18"/>
+        <v>if(board[3][3]!=0) column44.setText(String.valueOf(board[3][3]));</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finally fixed logic and display bug for btnDown
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:I19"/>
+      <selection activeCell="F21" sqref="F21:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,6 +778,78 @@
         <v>if(board[3][3]!=0) column44.setText(String.valueOf(board[3][3]));</v>
       </c>
     </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f>"if("&amp;F1&amp;".getText().equals("&amp;CHAR(34)&amp;"0"&amp;CHAR(34)&amp;")) "&amp;F1&amp;".setText(null);"</f>
+        <v>if(column11.getText().equals("0")) column11.setText(null);</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" ref="G21:I21" si="19">"if("&amp;G1&amp;".getText().equals("&amp;CHAR(34)&amp;"0"&amp;CHAR(34)&amp;")) "&amp;G1&amp;".setText(null);"</f>
+        <v>if(column12.getText().equals("0")) column12.setText(null);</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="19"/>
+        <v>if(column13.getText().equals("0")) column13.setText(null);</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="19"/>
+        <v>if(column14.getText().equals("0")) column14.setText(null);</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" ref="F22:I24" si="20">"if("&amp;F2&amp;".getText().equals("&amp;CHAR(34)&amp;"0"&amp;CHAR(34)&amp;")) "&amp;F2&amp;".setText(null);"</f>
+        <v>if(column21.getText().equals("0")) column21.setText(null);</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column22.getText().equals("0")) column22.setText(null);</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column23.getText().equals("0")) column23.setText(null);</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column24.getText().equals("0")) column24.setText(null);</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column31.getText().equals("0")) column31.setText(null);</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column32.getText().equals("0")) column32.setText(null);</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column33.getText().equals("0")) column33.setText(null);</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column34.getText().equals("0")) column34.setText(null);</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column41.getText().equals("0")) column41.setText(null);</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column42.getText().equals("0")) column42.setText(null);</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column43.getText().equals("0")) column43.setText(null);</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="20"/>
+        <v>if(column44.getText().equals("0")) column44.setText(null);</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add last added number highlighting
</commit_message>
<xml_diff>
--- a/views.xlsx
+++ b/views.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,6 +21,59 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="I31" sqref="F31:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +617,18 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="F6" t="str">
         <f>F1&amp;"=findViewById(R.id."&amp;F1&amp;");"</f>
         <v>column11=findViewById(R.id.column11);</v>
@@ -581,6 +647,18 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F7" t="str">
         <f t="shared" ref="F7:I9" si="8">F2&amp;"=findViewById(R.id."&amp;F2&amp;");"</f>
         <v>column21=findViewById(R.id.column21);</v>
@@ -599,6 +677,18 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" t="str">
         <f t="shared" si="8"/>
         <v>column31=findViewById(R.id.column31);</v>
@@ -617,6 +707,18 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" t="str">
         <f t="shared" si="8"/>
         <v>column41=findViewById(R.id.column41);</v>
@@ -920,6 +1022,78 @@
       <c r="I29" t="str">
         <f t="shared" si="26"/>
         <v>column44.getBackground().setColorFilter(null);</v>
+      </c>
+    </row>
+    <row r="31" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F31" t="str">
+        <f>"if(row=="&amp;LEFT(A6,1)&amp;" &amp;&amp; column=="&amp;RIGHT(A6,1)&amp;") "&amp;F1&amp;".getBackground().setColorFilter(Color.parseColor("&amp;CHAR(34)&amp;"#ECEFF1"&amp;CHAR(34)&amp;"), PorterDuff.Mode.ADD);"</f>
+        <v>if(row==0 &amp;&amp; column==0) column11.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" ref="G31:I31" si="27">"if(row=="&amp;LEFT(B6,1)&amp;" &amp;&amp; column=="&amp;RIGHT(B6,1)&amp;") "&amp;G1&amp;".getBackground().setColorFilter(Color.parseColor("&amp;CHAR(34)&amp;"#ECEFF1"&amp;CHAR(34)&amp;"), PorterDuff.Mode.ADD);"</f>
+        <v>if(row==0 &amp;&amp; column==1) column12.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="27"/>
+        <v>if(row==0 &amp;&amp; column==2) column13.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="27"/>
+        <v>if(row==0 &amp;&amp; column==3) column14.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F32" t="str">
+        <f t="shared" ref="F32:F34" si="28">"if(row=="&amp;LEFT(A7,1)&amp;" &amp;&amp; column=="&amp;RIGHT(A7,1)&amp;") "&amp;F2&amp;".getBackground().setColorFilter(Color.parseColor("&amp;CHAR(34)&amp;"#ECEFF1"&amp;CHAR(34)&amp;"), PorterDuff.Mode.ADD);"</f>
+        <v>if(row==1 &amp;&amp; column==0) column21.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" ref="G32:G34" si="29">"if(row=="&amp;LEFT(B7,1)&amp;" &amp;&amp; column=="&amp;RIGHT(B7,1)&amp;") "&amp;G2&amp;".getBackground().setColorFilter(Color.parseColor("&amp;CHAR(34)&amp;"#ECEFF1"&amp;CHAR(34)&amp;"), PorterDuff.Mode.ADD);"</f>
+        <v>if(row==1 &amp;&amp; column==1) column22.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" ref="H32:H34" si="30">"if(row=="&amp;LEFT(C7,1)&amp;" &amp;&amp; column=="&amp;RIGHT(C7,1)&amp;") "&amp;H2&amp;".getBackground().setColorFilter(Color.parseColor("&amp;CHAR(34)&amp;"#ECEFF1"&amp;CHAR(34)&amp;"), PorterDuff.Mode.ADD);"</f>
+        <v>if(row==1 &amp;&amp; column==2) column23.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" ref="I32:I34" si="31">"if(row=="&amp;LEFT(D7,1)&amp;" &amp;&amp; column=="&amp;RIGHT(D7,1)&amp;") "&amp;I2&amp;".getBackground().setColorFilter(Color.parseColor("&amp;CHAR(34)&amp;"#ECEFF1"&amp;CHAR(34)&amp;"), PorterDuff.Mode.ADD);"</f>
+        <v>if(row==1 &amp;&amp; column==3) column24.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33" t="str">
+        <f t="shared" si="28"/>
+        <v>if(row==2 &amp;&amp; column==0) column31.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="29"/>
+        <v>if(row==2 &amp;&amp; column==1) column32.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="30"/>
+        <v>if(row==2 &amp;&amp; column==2) column33.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="31"/>
+        <v>if(row==2 &amp;&amp; column==3) column34.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F34" t="str">
+        <f t="shared" si="28"/>
+        <v>if(row==3 &amp;&amp; column==0) column41.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="29"/>
+        <v>if(row==3 &amp;&amp; column==1) column42.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="30"/>
+        <v>if(row==3 &amp;&amp; column==2) column43.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="31"/>
+        <v>if(row==3 &amp;&amp; column==3) column44.getBackground().setColorFilter(Color.parseColor("#ECEFF1"), PorterDuff.Mode.ADD);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>